<commit_message>
More work done on the vcf reader
</commit_message>
<xml_diff>
--- a/VCardReader/Languages.xlsx
+++ b/VCardReader/Languages.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="216">
   <si>
     <t>AssistantLabel</t>
   </si>
@@ -95,9 +95,6 @@
     <t>Hoofdtelefoon bedrijf</t>
   </si>
   <si>
-    <t>DataFormatDataFormat</t>
-  </si>
-  <si>
     <t>dd-MM-yyyy</t>
   </si>
   <si>
@@ -119,42 +116,6 @@
     <t>Volledige naam</t>
   </si>
   <si>
-    <t>Email1DisplayNameLabel</t>
-  </si>
-  <si>
-    <t>E-mail - weergeven naam 1</t>
-  </si>
-  <si>
-    <t>Email1EmailAddressLabel</t>
-  </si>
-  <si>
-    <t>E-mail</t>
-  </si>
-  <si>
-    <t>Email2DisplayNameLabel</t>
-  </si>
-  <si>
-    <t>E-mail - weergeven naam 2</t>
-  </si>
-  <si>
-    <t>Email2EmailAddressLabel</t>
-  </si>
-  <si>
-    <t>E-mail 2</t>
-  </si>
-  <si>
-    <t>Email3DisplayNameLabel</t>
-  </si>
-  <si>
-    <t>E-mail - weergeven naam 3</t>
-  </si>
-  <si>
-    <t>Email3EmailAddressLabel</t>
-  </si>
-  <si>
-    <t>E-mail 3</t>
-  </si>
-  <si>
     <t>FunctionLabel</t>
   </si>
   <si>
@@ -350,12 +311,6 @@
     <t>E-mail Anzeige als</t>
   </si>
   <si>
-    <t>E-mail 2 Anzeige als</t>
-  </si>
-  <si>
-    <t>E-mail 3 Anzeige als</t>
-  </si>
-  <si>
     <t>Job title</t>
   </si>
   <si>
@@ -458,21 +413,6 @@
     <t>Afficher la messagerie comme</t>
   </si>
   <si>
-    <t>Adresse de messagerie</t>
-  </si>
-  <si>
-    <t>Afficher la messagerie comme 2</t>
-  </si>
-  <si>
-    <t>Adresse de messagerie 2</t>
-  </si>
-  <si>
-    <t>Afficher la messagerie comme 3</t>
-  </si>
-  <si>
-    <t>Adresse de messagerie 3</t>
-  </si>
-  <si>
     <t>Fonction</t>
   </si>
   <si>
@@ -578,12 +518,6 @@
     <t>E-mail display as</t>
   </si>
   <si>
-    <t>E-mail 2 display as</t>
-  </si>
-  <si>
-    <t>E-mail 3 display as</t>
-  </si>
-  <si>
     <t>First name</t>
   </si>
   <si>
@@ -636,13 +570,115 @@
   </si>
   <si>
     <t>Normally Outlook will use the subject of a MSG object as it's filename. Invalid characters are replaced by spaces. When there is no subject outlook uses "Nameless" as default</t>
+  </si>
+  <si>
+    <t>DomesticAddressLabel</t>
+  </si>
+  <si>
+    <t>Domestic address</t>
+  </si>
+  <si>
+    <t>InternationalAddressLabel</t>
+  </si>
+  <si>
+    <t>International address</t>
+  </si>
+  <si>
+    <t>Internaltionaal adres</t>
+  </si>
+  <si>
+    <t>International adresse</t>
+  </si>
+  <si>
+    <t>PostalAddressLabel</t>
+  </si>
+  <si>
+    <t>Postal address</t>
+  </si>
+  <si>
+    <t>Postbus adres</t>
+  </si>
+  <si>
+    <t>Postal anschrift</t>
+  </si>
+  <si>
+    <t>International anschrift</t>
+  </si>
+  <si>
+    <t>Postal adresse</t>
+  </si>
+  <si>
+    <t>ParcelAddressLabel</t>
+  </si>
+  <si>
+    <t>Parcel address</t>
+  </si>
+  <si>
+    <t>Pakjes adres</t>
+  </si>
+  <si>
+    <t>Parcel anschrift</t>
+  </si>
+  <si>
+    <t>Parcel adresse</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>ModemTelephoneNumberLabel</t>
+  </si>
+  <si>
+    <t>Modem</t>
+  </si>
+  <si>
+    <t>VideoTelephoneNumberLabel</t>
+  </si>
+  <si>
+    <t>Video</t>
+  </si>
+  <si>
+    <t>VoiceTelephoneNumberLabel</t>
+  </si>
+  <si>
+    <t>Voice</t>
+  </si>
+  <si>
+    <t>BBSTelephoneNumberLabel</t>
+  </si>
+  <si>
+    <t>BBS</t>
+  </si>
+  <si>
+    <t>EmailDisplayNameLabel</t>
+  </si>
+  <si>
+    <t>E-mail - weergeven naam</t>
+  </si>
+  <si>
+    <t>DataFormat</t>
+  </si>
+  <si>
+    <t>CategoriesLabel</t>
+  </si>
+  <si>
+    <t>Categories</t>
+  </si>
+  <si>
+    <t>Categoriëen</t>
+  </si>
+  <si>
+    <t>Kategorien</t>
+  </si>
+  <si>
+    <t>Catégories</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -650,16 +686,29 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -667,17 +716,36 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Calculation" xfId="1" builtinId="22"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -956,36 +1024,39 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F47"/>
+  <dimension ref="A1:F51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C39" sqref="C39"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="B51" sqref="A51:B51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="60.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="36.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.5703125" customWidth="1"/>
+    <col min="3" max="3" width="25.28515625" customWidth="1"/>
     <col min="4" max="4" width="24.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="29.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="29.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>90</v>
-      </c>
-      <c r="B1" t="s">
-        <v>93</v>
-      </c>
-      <c r="C1" t="s">
-        <v>92</v>
-      </c>
-      <c r="D1" t="s">
-        <v>91</v>
-      </c>
-      <c r="E1" t="s">
-        <v>94</v>
+    <row r="1" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>199</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -993,16 +1064,16 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>171</v>
+        <v>151</v>
       </c>
       <c r="C2" t="s">
         <v>1</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>95</v>
+        <v>82</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>131</v>
+        <v>116</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -1010,16 +1081,16 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>171</v>
+        <v>151</v>
       </c>
       <c r="C3" t="s">
         <v>1</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>95</v>
+        <v>82</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>132</v>
+        <v>117</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -1044,16 +1115,16 @@
         <v>5</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>172</v>
+        <v>152</v>
       </c>
       <c r="C5" t="s">
         <v>6</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>133</v>
+        <v>118</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -1061,16 +1132,16 @@
         <v>7</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>173</v>
+        <v>153</v>
       </c>
       <c r="C6" t="s">
         <v>8</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>97</v>
+        <v>84</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>134</v>
+        <v>119</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -1078,16 +1149,16 @@
         <v>9</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>174</v>
+        <v>154</v>
       </c>
       <c r="C7" t="s">
         <v>10</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>98</v>
+        <v>85</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>135</v>
+        <v>120</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -1095,16 +1166,16 @@
         <v>11</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>175</v>
+        <v>155</v>
       </c>
       <c r="C8" t="s">
         <v>12</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>99</v>
+        <v>86</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>136</v>
+        <v>121</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -1112,16 +1183,16 @@
         <v>13</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>176</v>
+        <v>156</v>
       </c>
       <c r="C9" t="s">
         <v>14</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>100</v>
+        <v>87</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>137</v>
+        <v>122</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -1129,16 +1200,16 @@
         <v>15</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>177</v>
+        <v>157</v>
       </c>
       <c r="C10" t="s">
         <v>16</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>101</v>
+        <v>88</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>138</v>
+        <v>123</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -1146,16 +1217,16 @@
         <v>17</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>102</v>
+        <v>89</v>
       </c>
       <c r="C11" t="s">
         <v>18</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>102</v>
+        <v>89</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>102</v>
+        <v>89</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -1163,16 +1234,16 @@
         <v>19</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>178</v>
+        <v>158</v>
       </c>
       <c r="C12" t="s">
         <v>20</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>103</v>
+        <v>90</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>139</v>
+        <v>124</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -1180,606 +1251,675 @@
         <v>21</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>179</v>
+        <v>159</v>
       </c>
       <c r="C13" t="s">
         <v>22</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>104</v>
+        <v>91</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>140</v>
+        <v>125</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>210</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="C14" t="s">
         <v>23</v>
       </c>
-      <c r="B14" s="1" t="s">
-        <v>180</v>
-      </c>
-      <c r="C14" t="s">
-        <v>24</v>
-      </c>
       <c r="D14" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>201</v>
+        <v>179</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C15" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F15" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>26</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="C16" t="s">
         <v>27</v>
       </c>
-      <c r="B16" s="1" t="s">
-        <v>181</v>
-      </c>
-      <c r="C16" t="s">
+      <c r="D16" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="F16" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
         <v>28</v>
       </c>
-      <c r="D16" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="F16" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+      <c r="B17" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="C17" t="s">
         <v>29</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="D17" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>182</v>
-      </c>
-      <c r="C17" t="s">
-        <v>30</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>31</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>183</v>
       </c>
       <c r="C18" t="s">
+        <v>35</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>208</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="C19" t="s">
+        <v>209</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>30</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="C20" t="s">
+        <v>31</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
         <v>32</v>
       </c>
-      <c r="D18" s="1" t="s">
+      <c r="B21" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="C21" t="s">
+        <v>33</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>34</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="C22" t="s">
+        <v>35</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>36</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="C23" t="s">
+        <v>37</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>38</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="C24" t="s">
+        <v>39</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>40</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="C25" t="s">
+        <v>41</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>42</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C26" t="s">
+        <v>43</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>44</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="C27" t="s">
+        <v>45</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>184</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="C28" t="s">
+        <v>186</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>46</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C29" t="s">
+        <v>47</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>48</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="C30" t="s">
+        <v>49</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="F30" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>50</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="C31" t="s">
+        <v>51</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>52</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="C32" t="s">
+        <v>53</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>54</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="C33" t="s">
+        <v>55</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>194</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="C34" t="s">
+        <v>196</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>188</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="C35" t="s">
+        <v>190</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>56</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="C36" t="s">
+        <v>53</v>
+      </c>
+      <c r="D36" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="E18" s="1" t="s">
+      <c r="E36" s="1" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>57</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="C37" t="s">
+        <v>58</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>59</v>
+      </c>
+      <c r="B38" s="1" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>33</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C19" t="s">
-        <v>34</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="E19" s="1" t="s">
+      <c r="C38" t="s">
+        <v>60</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>61</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C39" t="s">
+        <v>62</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>63</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="C40" t="s">
+        <v>64</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="E40" s="1" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>35</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="C20" t="s">
-        <v>36</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="E20" s="1" t="s">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>65</v>
+      </c>
+      <c r="B41" s="1" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>37</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="C21" t="s">
-        <v>38</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="E21" s="1" t="s">
+      <c r="C41" t="s">
+        <v>66</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>67</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="C42" t="s">
+        <v>68</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="E42" s="1" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>39</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>185</v>
-      </c>
-      <c r="C22" t="s">
-        <v>40</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="E22" s="1" t="s">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>69</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C43" t="s">
+        <v>70</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="E43" s="1" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>41</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="C23" t="s">
-        <v>42</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="E23" s="1" t="s">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>71</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="C44" t="s">
+        <v>72</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="E44" s="1" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>43</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="C24" t="s">
-        <v>44</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="E24" s="1" t="s">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>73</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="C45" t="s">
+        <v>74</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="E45" s="1" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>45</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>186</v>
-      </c>
-      <c r="C25" t="s">
-        <v>46</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="E25" s="1" t="s">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>75</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="C46" t="s">
+        <v>76</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="E46" s="1" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>47</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>187</v>
-      </c>
-      <c r="C26" t="s">
-        <v>48</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="E26" s="1" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>49</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>188</v>
-      </c>
-      <c r="C27" t="s">
-        <v>50</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="E27" s="1" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>51</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="C28" t="s">
-        <v>52</v>
-      </c>
-      <c r="D28" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="E28" s="1" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>53</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>190</v>
-      </c>
-      <c r="C29" t="s">
-        <v>54</v>
-      </c>
-      <c r="D29" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="E29" s="1" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>55</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="C30" t="s">
-        <v>56</v>
-      </c>
-      <c r="D30" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="E30" s="1" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>57</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="C31" t="s">
-        <v>58</v>
-      </c>
-      <c r="D31" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="E31" s="1" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>59</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="C32" t="s">
-        <v>60</v>
-      </c>
-      <c r="D32" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="E32" s="1" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>61</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>192</v>
-      </c>
-      <c r="C33" t="s">
-        <v>62</v>
-      </c>
-      <c r="D33" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="E33" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="F33" t="s">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>200</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="E47" s="1" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>202</v>
+      </c>
+      <c r="B48" s="1" t="s">
         <v>203</v>
       </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>63</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>193</v>
-      </c>
-      <c r="C34" t="s">
-        <v>64</v>
-      </c>
-      <c r="D34" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="E34" s="1" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>65</v>
-      </c>
-      <c r="B35" s="1" t="s">
-        <v>194</v>
-      </c>
-      <c r="C35" t="s">
-        <v>66</v>
-      </c>
-      <c r="D35" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="E35" s="1" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>67</v>
-      </c>
-      <c r="B36" s="1" t="s">
-        <v>195</v>
-      </c>
-      <c r="C36" t="s">
-        <v>68</v>
-      </c>
-      <c r="D36" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="E36" s="1" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>69</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>194</v>
-      </c>
-      <c r="C37" t="s">
-        <v>66</v>
-      </c>
-      <c r="D37" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="E37" s="1" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>70</v>
-      </c>
-      <c r="B38" s="1" t="s">
-        <v>196</v>
-      </c>
-      <c r="C38" t="s">
-        <v>71</v>
-      </c>
-      <c r="D38" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="E38" s="1" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>72</v>
-      </c>
-      <c r="B39" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="C39" t="s">
-        <v>73</v>
-      </c>
-      <c r="D39" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="E39" s="1" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>74</v>
-      </c>
-      <c r="B40" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="C40" t="s">
-        <v>75</v>
-      </c>
-      <c r="D40" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="E40" s="1" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>76</v>
-      </c>
-      <c r="B41" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="C41" t="s">
-        <v>77</v>
-      </c>
-      <c r="D41" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="E41" s="1" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>78</v>
-      </c>
-      <c r="B42" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="C42" t="s">
-        <v>79</v>
-      </c>
-      <c r="D42" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="E42" s="1" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>80</v>
-      </c>
-      <c r="B43" s="1" t="s">
-        <v>198</v>
-      </c>
-      <c r="C43" t="s">
-        <v>81</v>
-      </c>
-      <c r="D43" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="E43" s="1" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
-        <v>82</v>
-      </c>
-      <c r="B44" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="C44" t="s">
-        <v>83</v>
-      </c>
-      <c r="D44" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="E44" s="1" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
-        <v>84</v>
-      </c>
-      <c r="B45" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="C45" t="s">
-        <v>85</v>
-      </c>
-      <c r="D45" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="E45" s="1" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
-        <v>86</v>
-      </c>
-      <c r="B46" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="C46" t="s">
-        <v>87</v>
-      </c>
-      <c r="D46" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="E46" s="1" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
-        <v>88</v>
-      </c>
-      <c r="B47" s="1" t="s">
-        <v>200</v>
-      </c>
-      <c r="C47" t="s">
-        <v>89</v>
-      </c>
-      <c r="D47" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="E47" s="1" t="s">
-        <v>170</v>
+      <c r="C48" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="E48" s="1" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>204</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="E49" s="1" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>206</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="E50" s="1" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>211</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="E51" s="1" t="s">
+        <v>215</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>